<commit_message>
added plotting text, dynamic updating on geocoder, but still bug in analysis
</commit_message>
<xml_diff>
--- a/RGC.xlsx
+++ b/RGC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giddu/Documents/Jobs/Cohanzick/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giddu/Documents/Jobs/Cohanzick/kawasakininja/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842E3DC8-58D7-9B4D-ABAA-40AF084529DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4800839-8E81-C64A-A9BF-32E5EF49D91A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{E5BEF27E-CD2A-E245-9908-8CA338D21673}"/>
   </bookViews>
@@ -5369,7 +5369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5393,14 +5393,6 @@
     <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -5411,6 +5403,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5726,10 +5722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07732F56-0CB8-FD4C-BE27-C1F8C452A0E7}">
-  <dimension ref="A1:K571"/>
+  <dimension ref="A1:K570"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K574" sqref="K574"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A546" workbookViewId="0">
+      <selection activeCell="A569" sqref="A569:XFD569"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19111,7 +19107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="569" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:11" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A569" s="3" t="s">
         <v>1740</v>
       </c>
@@ -19124,14 +19120,14 @@
       <c r="D569" s="3" t="s">
         <v>1743</v>
       </c>
-      <c r="E569" s="11">
-        <v>1</v>
-      </c>
-      <c r="F569" s="11"/>
-      <c r="G569" s="11"/>
-      <c r="H569" s="11"/>
-      <c r="I569" s="12"/>
-      <c r="J569" s="12"/>
+      <c r="E569" s="15">
+        <v>1</v>
+      </c>
+      <c r="F569" s="15"/>
+      <c r="G569" s="15"/>
+      <c r="H569" s="15"/>
+      <c r="I569" s="16"/>
+      <c r="J569" s="16"/>
       <c r="K569" s="2">
         <v>1</v>
       </c>
@@ -19140,27 +19136,14 @@
       <c r="A570" s="3"/>
       <c r="B570" s="3"/>
       <c r="C570" s="3"/>
-      <c r="D570" s="13"/>
-      <c r="E570" s="14"/>
-      <c r="F570" s="14"/>
-      <c r="G570" s="14"/>
-      <c r="H570" s="14"/>
+      <c r="D570" s="11"/>
+      <c r="E570" s="12"/>
+      <c r="F570" s="13"/>
+      <c r="G570" s="13"/>
+      <c r="H570" s="13"/>
       <c r="I570" s="14"/>
       <c r="J570" s="14"/>
       <c r="K570" s="2"/>
-    </row>
-    <row r="571" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A571" s="3"/>
-      <c r="B571" s="3"/>
-      <c r="C571" s="3"/>
-      <c r="D571" s="15"/>
-      <c r="E571" s="16"/>
-      <c r="F571" s="17"/>
-      <c r="G571" s="17"/>
-      <c r="H571" s="17"/>
-      <c r="I571" s="18"/>
-      <c r="J571" s="18"/>
-      <c r="K571" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>